<commit_message>
Use NuGet package Microsoft.Data.Sqlite to access sqlite databases. Tidy inconsistent use of "TOS" in Canola validation.
</commit_message>
<xml_diff>
--- a/Tests/Validation/Canola/Wagga2008.xlsx
+++ b/Tests/Validation/Canola/Wagga2008.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB543AAD-EA18-4FCE-9450-99E67676BABE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90C95E-C28C-4AF6-A407-17C92EBE8BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="225" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="670" yWindow="1520" windowWidth="18530" windowHeight="8810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="3" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="52">
   <si>
     <t>HAr GAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HI + leaf</t>
   </si>
   <si>
     <t>Low</t>
@@ -101,9 +98,6 @@
     <t>Popn</t>
   </si>
   <si>
-    <t>TOS</t>
-  </si>
-  <si>
     <t>AV_Garnet</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>HAr GAIError</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HI + leafError</t>
   </si>
   <si>
     <t/>
@@ -192,6 +183,15 @@
   </si>
   <si>
     <t>WaggaCR2008CvATR_Marlin</t>
+  </si>
+  <si>
+    <t>HI + leafError</t>
+  </si>
+  <si>
+    <t>HI + leaf</t>
+  </si>
+  <si>
+    <t>TOS_index</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -269,10 +269,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,166 +554,165 @@
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AK86" sqref="AK86:AK100"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.81640625" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1796875" customWidth="1"/>
     <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.1796875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="23" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.26953125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="20" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="7" t="s">
+      <c r="P1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
-        <v>13</v>
       </c>
       <c r="W1" t="s">
         <v>0</v>
       </c>
       <c r="X1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="Z1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>29</v>
-      </c>
       <c r="AL1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>C2&amp;B2&amp;"Cv"&amp;D2&amp;"Treat"&amp;E2</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -724,13 +721,13 @@
         <v>2008</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2">
         <v>67</v>
@@ -745,7 +742,7 @@
         <v>39611</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="10">
+      <c r="K2">
         <f>I2-H2</f>
         <v>44</v>
       </c>
@@ -797,7 +794,7 @@
       <c r="AK2" s="3"/>
       <c r="AL2" s="3"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3&amp;B3&amp;"Cv"&amp;D3&amp;"Treat"&amp;E3</f>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -806,13 +803,13 @@
         <v>2008</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>67</v>
@@ -827,12 +824,12 @@
         <v>39633</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="10">
+      <c r="K3">
         <f t="shared" ref="K3:K66" si="1">I3-H3</f>
         <v>66</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M3" s="5">
         <v>187.38749999999999</v>
@@ -877,7 +874,7 @@
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -886,13 +883,13 @@
         <v>2008</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>67</v>
@@ -907,7 +904,7 @@
         <v>39640</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="10">
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -959,7 +956,7 @@
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -968,13 +965,13 @@
         <v>2008</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>67</v>
@@ -989,7 +986,7 @@
         <v>39655</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="10">
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -1041,7 +1038,7 @@
       <c r="AK5" s="3"/>
       <c r="AL5" s="3"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1050,13 +1047,13 @@
         <v>2008</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>67</v>
@@ -1071,7 +1068,7 @@
         <v>39668</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="10">
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -1123,7 +1120,7 @@
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1132,13 +1129,13 @@
         <v>2008</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7">
         <v>67</v>
@@ -1153,7 +1150,7 @@
         <v>39699</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="10">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
@@ -1205,7 +1202,7 @@
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatHigh</v>
@@ -1214,13 +1211,13 @@
         <v>2008</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F8">
         <v>67</v>
@@ -1234,10 +1231,10 @@
       <c r="I8" s="1">
         <v>39762</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8">
         <v>9</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
@@ -1316,7 +1313,7 @@
         <v>1.5082910959437631E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1325,13 +1322,13 @@
         <v>2008</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9">
         <v>48</v>
@@ -1346,7 +1343,7 @@
         <v>39611</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="10">
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -1357,7 +1354,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -1384,7 +1381,7 @@
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1393,13 +1390,13 @@
         <v>2008</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10">
         <v>48</v>
@@ -1414,12 +1411,12 @@
         <v>39633</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="10">
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M10" s="5">
         <v>28.410648148148152</v>
@@ -1429,7 +1426,7 @@
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -1458,7 +1455,7 @@
       <c r="AK10" s="3"/>
       <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1467,13 +1464,13 @@
         <v>2008</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11">
         <v>48</v>
@@ -1488,7 +1485,7 @@
         <v>39640</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="10">
+      <c r="K11">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
@@ -1540,7 +1537,7 @@
       <c r="AK11" s="3"/>
       <c r="AL11" s="3"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1549,13 +1546,13 @@
         <v>2008</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12">
         <v>48</v>
@@ -1570,7 +1567,7 @@
         <v>39655</v>
       </c>
       <c r="J12" s="1"/>
-      <c r="K12" s="10">
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
@@ -1622,7 +1619,7 @@
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1631,13 +1628,13 @@
         <v>2008</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13">
         <v>48</v>
@@ -1652,7 +1649,7 @@
         <v>39668</v>
       </c>
       <c r="J13" s="1"/>
-      <c r="K13" s="10">
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -1704,7 +1701,7 @@
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1713,13 +1710,13 @@
         <v>2008</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14">
         <v>48</v>
@@ -1734,7 +1731,7 @@
         <v>39708</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="10">
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>132</v>
       </c>
@@ -1786,7 +1783,7 @@
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLate</v>
@@ -1795,13 +1792,13 @@
         <v>2008</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F15">
         <v>48</v>
@@ -1815,10 +1812,10 @@
       <c r="I15" s="1">
         <v>39763</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15">
         <v>9</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>187</v>
       </c>
@@ -1897,7 +1894,7 @@
         <v>7.3689311541742753E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -1906,13 +1903,13 @@
         <v>2008</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>27</v>
@@ -1927,7 +1924,7 @@
         <v>39611</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="10">
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -1979,7 +1976,7 @@
       <c r="AK16" s="3"/>
       <c r="AL16" s="3"/>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -1988,13 +1985,13 @@
         <v>2008</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>27</v>
@@ -2009,12 +2006,12 @@
         <v>39633</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="10">
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M17" s="5">
         <v>113.0895</v>
@@ -2059,7 +2056,7 @@
       <c r="AK17" s="3"/>
       <c r="AL17" s="3"/>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2068,13 +2065,13 @@
         <v>2008</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>27</v>
@@ -2089,7 +2086,7 @@
         <v>39640</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="10">
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -2141,7 +2138,7 @@
       <c r="AK18" s="3"/>
       <c r="AL18" s="3"/>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2150,13 +2147,13 @@
         <v>2008</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>27</v>
@@ -2171,7 +2168,7 @@
         <v>39655</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="K19" s="10">
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -2223,7 +2220,7 @@
       <c r="AK19" s="3"/>
       <c r="AL19" s="3"/>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2232,13 +2229,13 @@
         <v>2008</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>27</v>
@@ -2253,7 +2250,7 @@
         <v>39668</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="10">
+      <c r="K20">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -2305,7 +2302,7 @@
       <c r="AK20" s="3"/>
       <c r="AL20" s="3"/>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2314,13 +2311,13 @@
         <v>2008</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>27</v>
@@ -2335,7 +2332,7 @@
         <v>39687</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="K21" s="10">
+      <c r="K21">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
@@ -2387,7 +2384,7 @@
       <c r="AK21" s="3"/>
       <c r="AL21" s="3"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatLow</v>
@@ -2396,13 +2393,13 @@
         <v>2008</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>27</v>
@@ -2416,10 +2413,10 @@
       <c r="I22" s="1">
         <v>39762</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22">
         <v>9</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
@@ -2498,7 +2495,7 @@
         <v>2.4262733164717942E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2507,13 +2504,13 @@
         <v>2008</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23">
         <v>48</v>
@@ -2528,7 +2525,7 @@
         <v>39611</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="10">
+      <c r="K23">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -2580,7 +2577,7 @@
       <c r="AK23" s="3"/>
       <c r="AL23" s="3"/>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2589,13 +2586,13 @@
         <v>2008</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F24">
         <v>48</v>
@@ -2610,12 +2607,12 @@
         <v>39633</v>
       </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="10">
+      <c r="K24">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M24" s="5">
         <v>167.26512499999998</v>
@@ -2660,7 +2657,7 @@
       <c r="AK24" s="3"/>
       <c r="AL24" s="3"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2669,13 +2666,13 @@
         <v>2008</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <v>48</v>
@@ -2690,7 +2687,7 @@
         <v>39640</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="10">
+      <c r="K25">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -2742,7 +2739,7 @@
       <c r="AK25" s="3"/>
       <c r="AL25" s="3"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2751,13 +2748,13 @@
         <v>2008</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26">
         <v>48</v>
@@ -2772,7 +2769,7 @@
         <v>39655</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="10">
+      <c r="K26">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -2824,7 +2821,7 @@
       <c r="AK26" s="3"/>
       <c r="AL26" s="3"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2833,13 +2830,13 @@
         <v>2008</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27">
         <v>48</v>
@@ -2854,7 +2851,7 @@
         <v>39668</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="10">
+      <c r="K27">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -2906,7 +2903,7 @@
       <c r="AK27" s="3"/>
       <c r="AL27" s="3"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2915,13 +2912,13 @@
         <v>2008</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28">
         <v>48</v>
@@ -2936,7 +2933,7 @@
         <v>39692</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="K28" s="10">
+      <c r="K28">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
@@ -2988,7 +2985,7 @@
       <c r="AK28" s="3"/>
       <c r="AL28" s="3"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008Cv46Y78TreatMid</v>
@@ -2997,13 +2994,13 @@
         <v>2008</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29">
         <v>48</v>
@@ -3017,10 +3014,10 @@
       <c r="I29" s="1">
         <v>39762</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29">
         <v>9</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
@@ -3099,7 +3096,7 @@
         <v>1.6341572459386597E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3108,13 +3105,13 @@
         <v>2008</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F30">
         <v>67</v>
@@ -3129,7 +3126,7 @@
         <v>39611</v>
       </c>
       <c r="J30" s="1"/>
-      <c r="K30" s="10">
+      <c r="K30">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -3181,7 +3178,7 @@
       <c r="AK30" s="3"/>
       <c r="AL30" s="3"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3190,13 +3187,13 @@
         <v>2008</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31">
         <v>67</v>
@@ -3211,12 +3208,12 @@
         <v>39633</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="10">
+      <c r="K31">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M31" s="5">
         <v>187.38749999999996</v>
@@ -3261,7 +3258,7 @@
       <c r="AK31" s="3"/>
       <c r="AL31" s="3"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3270,13 +3267,13 @@
         <v>2008</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F32">
         <v>67</v>
@@ -3291,7 +3288,7 @@
         <v>39640</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="10">
+      <c r="K32">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -3343,7 +3340,7 @@
       <c r="AK32" s="3"/>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3352,13 +3349,13 @@
         <v>2008</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <v>67</v>
@@ -3373,7 +3370,7 @@
         <v>39655</v>
       </c>
       <c r="J33" s="1"/>
-      <c r="K33" s="10">
+      <c r="K33">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -3425,7 +3422,7 @@
       <c r="AK33" s="3"/>
       <c r="AL33" s="3"/>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3434,13 +3431,13 @@
         <v>2008</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34">
         <v>67</v>
@@ -3455,7 +3452,7 @@
         <v>39668</v>
       </c>
       <c r="J34" s="1"/>
-      <c r="K34" s="10">
+      <c r="K34">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -3507,7 +3504,7 @@
       <c r="AK34" s="3"/>
       <c r="AL34" s="3"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3516,13 +3513,13 @@
         <v>2008</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35">
         <v>67</v>
@@ -3537,7 +3534,7 @@
         <v>39684</v>
       </c>
       <c r="J35" s="1"/>
-      <c r="K35" s="10">
+      <c r="K35">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
@@ -3589,7 +3586,7 @@
       <c r="AK35" s="3"/>
       <c r="AL35" s="3"/>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatHigh</v>
@@ -3598,13 +3595,13 @@
         <v>2008</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36">
         <v>67</v>
@@ -3618,10 +3615,10 @@
       <c r="I36" s="1">
         <v>39748</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36">
         <v>9</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36">
         <f t="shared" si="1"/>
         <v>181</v>
       </c>
@@ -3700,7 +3697,7 @@
         <v>1.594680804767807E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3709,13 +3706,13 @@
         <v>2008</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F37">
         <v>48</v>
@@ -3730,7 +3727,7 @@
         <v>39611</v>
       </c>
       <c r="J37" s="1"/>
-      <c r="K37" s="10">
+      <c r="K37">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -3741,7 +3738,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
@@ -3768,7 +3765,7 @@
       <c r="AK37" s="3"/>
       <c r="AL37" s="3"/>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3777,13 +3774,13 @@
         <v>2008</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F38">
         <v>48</v>
@@ -3798,12 +3795,12 @@
         <v>39633</v>
       </c>
       <c r="J38" s="1"/>
-      <c r="K38" s="10">
+      <c r="K38">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M38" s="5">
         <v>22.952546296296294</v>
@@ -3813,7 +3810,7 @@
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
@@ -3842,7 +3839,7 @@
       <c r="AK38" s="3"/>
       <c r="AL38" s="3"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3851,13 +3848,13 @@
         <v>2008</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F39">
         <v>48</v>
@@ -3872,7 +3869,7 @@
         <v>39640</v>
       </c>
       <c r="J39" s="1"/>
-      <c r="K39" s="10">
+      <c r="K39">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
@@ -3924,7 +3921,7 @@
       <c r="AK39" s="3"/>
       <c r="AL39" s="3"/>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -3933,13 +3930,13 @@
         <v>2008</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F40">
         <v>48</v>
@@ -3954,7 +3951,7 @@
         <v>39655</v>
       </c>
       <c r="J40" s="1"/>
-      <c r="K40" s="10">
+      <c r="K40">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
@@ -4006,7 +4003,7 @@
       <c r="AK40" s="3"/>
       <c r="AL40" s="3"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4015,13 +4012,13 @@
         <v>2008</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F41">
         <v>48</v>
@@ -4036,7 +4033,7 @@
         <v>39668</v>
       </c>
       <c r="J41" s="1"/>
-      <c r="K41" s="10">
+      <c r="K41">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -4088,7 +4085,7 @@
       <c r="AK41" s="3"/>
       <c r="AL41" s="3"/>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4097,13 +4094,13 @@
         <v>2008</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F42">
         <v>48</v>
@@ -4118,7 +4115,7 @@
         <v>39699</v>
       </c>
       <c r="J42" s="1"/>
-      <c r="K42" s="10">
+      <c r="K42">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
@@ -4170,7 +4167,7 @@
       <c r="AK42" s="3"/>
       <c r="AL42" s="3"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLate</v>
@@ -4179,13 +4176,13 @@
         <v>2008</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F43">
         <v>48</v>
@@ -4199,10 +4196,10 @@
       <c r="I43" s="1">
         <v>39763</v>
       </c>
-      <c r="J43" s="10">
+      <c r="J43">
         <v>9</v>
       </c>
-      <c r="K43" s="10">
+      <c r="K43">
         <f t="shared" si="1"/>
         <v>187</v>
       </c>
@@ -4281,7 +4278,7 @@
         <v>3.0796328121556358E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4290,13 +4287,13 @@
         <v>2008</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44">
         <v>27</v>
@@ -4311,7 +4308,7 @@
         <v>39611</v>
       </c>
       <c r="J44" s="1"/>
-      <c r="K44" s="10">
+      <c r="K44">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -4363,7 +4360,7 @@
       <c r="AK44" s="3"/>
       <c r="AL44" s="3"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4372,13 +4369,13 @@
         <v>2008</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45">
         <v>27</v>
@@ -4393,12 +4390,12 @@
         <v>39633</v>
       </c>
       <c r="J45" s="1"/>
-      <c r="K45" s="10">
+      <c r="K45">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M45" s="5">
         <v>106.12406249999999</v>
@@ -4443,7 +4440,7 @@
       <c r="AK45" s="3"/>
       <c r="AL45" s="3"/>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4452,13 +4449,13 @@
         <v>2008</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F46">
         <v>27</v>
@@ -4473,7 +4470,7 @@
         <v>39640</v>
       </c>
       <c r="J46" s="1"/>
-      <c r="K46" s="10">
+      <c r="K46">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -4525,7 +4522,7 @@
       <c r="AK46" s="3"/>
       <c r="AL46" s="3"/>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4534,13 +4531,13 @@
         <v>2008</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>27</v>
@@ -4555,7 +4552,7 @@
         <v>39655</v>
       </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="10">
+      <c r="K47">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -4607,7 +4604,7 @@
       <c r="AK47" s="3"/>
       <c r="AL47" s="3"/>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4616,13 +4613,13 @@
         <v>2008</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48">
         <v>27</v>
@@ -4637,7 +4634,7 @@
         <v>39668</v>
       </c>
       <c r="J48" s="1"/>
-      <c r="K48" s="10">
+      <c r="K48">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -4689,7 +4686,7 @@
       <c r="AK48" s="3"/>
       <c r="AL48" s="3"/>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4698,13 +4695,13 @@
         <v>2008</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49">
         <v>27</v>
@@ -4719,7 +4716,7 @@
         <v>39681</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="10">
+      <c r="K49">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
@@ -4771,7 +4768,7 @@
       <c r="AK49" s="3"/>
       <c r="AL49" s="3"/>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatLow</v>
@@ -4780,13 +4777,13 @@
         <v>2008</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50">
         <v>27</v>
@@ -4800,10 +4797,10 @@
       <c r="I50" s="1">
         <v>39748</v>
       </c>
-      <c r="J50" s="10">
+      <c r="J50">
         <v>9</v>
       </c>
-      <c r="K50" s="10">
+      <c r="K50">
         <f t="shared" si="1"/>
         <v>181</v>
       </c>
@@ -4882,7 +4879,7 @@
         <v>6.8418886233867415E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4891,13 +4888,13 @@
         <v>2008</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51">
         <v>48</v>
@@ -4912,7 +4909,7 @@
         <v>39611</v>
       </c>
       <c r="J51" s="1"/>
-      <c r="K51" s="10">
+      <c r="K51">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -4964,7 +4961,7 @@
       <c r="AK51" s="3"/>
       <c r="AL51" s="3"/>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -4973,13 +4970,13 @@
         <v>2008</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52">
         <v>48</v>
@@ -4994,12 +4991,12 @@
         <v>39633</v>
       </c>
       <c r="J52" s="1"/>
-      <c r="K52" s="10">
+      <c r="K52">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M52" s="5">
         <v>151.0124375</v>
@@ -5044,7 +5041,7 @@
       <c r="AK52" s="3"/>
       <c r="AL52" s="3"/>
     </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5053,13 +5050,13 @@
         <v>2008</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53">
         <v>48</v>
@@ -5074,7 +5071,7 @@
         <v>39640</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="10">
+      <c r="K53">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -5126,7 +5123,7 @@
       <c r="AK53" s="3"/>
       <c r="AL53" s="3"/>
     </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5135,13 +5132,13 @@
         <v>2008</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F54">
         <v>48</v>
@@ -5156,7 +5153,7 @@
         <v>39655</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="10">
+      <c r="K54">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -5208,7 +5205,7 @@
       <c r="AK54" s="3"/>
       <c r="AL54" s="3"/>
     </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5217,13 +5214,13 @@
         <v>2008</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55">
         <v>48</v>
@@ -5238,7 +5235,7 @@
         <v>39668</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="10">
+      <c r="K55">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -5290,7 +5287,7 @@
       <c r="AK55" s="3"/>
       <c r="AL55" s="3"/>
     </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5299,13 +5296,13 @@
         <v>2008</v>
       </c>
       <c r="C56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F56">
         <v>48</v>
@@ -5320,7 +5317,7 @@
         <v>39682</v>
       </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="10">
+      <c r="K56">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
@@ -5372,7 +5369,7 @@
       <c r="AK56" s="3"/>
       <c r="AL56" s="3"/>
     </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvAV_GarnetTreatMid</v>
@@ -5381,13 +5378,13 @@
         <v>2008</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57">
         <v>48</v>
@@ -5401,10 +5398,10 @@
       <c r="I57" s="1">
         <v>39748</v>
       </c>
-      <c r="J57" s="10">
+      <c r="J57">
         <v>9</v>
       </c>
-      <c r="K57" s="10">
+      <c r="K57">
         <f t="shared" si="1"/>
         <v>181</v>
       </c>
@@ -5483,7 +5480,7 @@
         <v>1.6838512560928193E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5492,13 +5489,13 @@
         <v>2008</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F58">
         <v>67</v>
@@ -5513,7 +5510,7 @@
         <v>39611</v>
       </c>
       <c r="J58" s="1"/>
-      <c r="K58" s="10">
+      <c r="K58">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
@@ -5565,7 +5562,7 @@
       <c r="AK58" s="3"/>
       <c r="AL58" s="3"/>
     </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5574,13 +5571,13 @@
         <v>2008</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F59">
         <v>67</v>
@@ -5595,12 +5592,12 @@
         <v>39633</v>
       </c>
       <c r="J59" s="1"/>
-      <c r="K59" s="10">
+      <c r="K59">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M59" s="5">
         <v>107.67193750000001</v>
@@ -5645,7 +5642,7 @@
       <c r="AK59" s="3"/>
       <c r="AL59" s="3"/>
     </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5654,13 +5651,13 @@
         <v>2008</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60">
         <v>67</v>
@@ -5675,7 +5672,7 @@
         <v>39640</v>
       </c>
       <c r="J60" s="1"/>
-      <c r="K60" s="10">
+      <c r="K60">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
@@ -5727,7 +5724,7 @@
       <c r="AK60" s="3"/>
       <c r="AL60" s="3"/>
     </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5736,13 +5733,13 @@
         <v>2008</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61">
         <v>67</v>
@@ -5757,7 +5754,7 @@
         <v>39655</v>
       </c>
       <c r="J61" s="1"/>
-      <c r="K61" s="10">
+      <c r="K61">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
@@ -5809,7 +5806,7 @@
       <c r="AK61" s="3"/>
       <c r="AL61" s="3"/>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5818,13 +5815,13 @@
         <v>2008</v>
       </c>
       <c r="C62" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F62">
         <v>67</v>
@@ -5839,7 +5836,7 @@
         <v>39668</v>
       </c>
       <c r="J62" s="1"/>
-      <c r="K62" s="10">
+      <c r="K62">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -5891,7 +5888,7 @@
       <c r="AK62" s="3"/>
       <c r="AL62" s="3"/>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5900,13 +5897,13 @@
         <v>2008</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63">
         <v>67</v>
@@ -5921,7 +5918,7 @@
         <v>39687</v>
       </c>
       <c r="J63" s="1"/>
-      <c r="K63" s="10">
+      <c r="K63">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
@@ -5973,7 +5970,7 @@
       <c r="AK63" s="3"/>
       <c r="AL63" s="3"/>
     </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatHigh</v>
@@ -5982,13 +5979,13 @@
         <v>2008</v>
       </c>
       <c r="C64" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F64">
         <v>67</v>
@@ -6002,10 +5999,10 @@
       <c r="I64" s="1">
         <v>39749</v>
       </c>
-      <c r="J64" s="10">
+      <c r="J64">
         <v>9</v>
       </c>
-      <c r="K64" s="10">
+      <c r="K64">
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
@@ -6084,7 +6081,7 @@
         <v>1.8344854302389708E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6093,13 +6090,13 @@
         <v>2008</v>
       </c>
       <c r="C65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E65" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F65">
         <v>48</v>
@@ -6114,7 +6111,7 @@
         <v>39611</v>
       </c>
       <c r="J65" s="1"/>
-      <c r="K65" s="10">
+      <c r="K65">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -6125,7 +6122,7 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
@@ -6152,7 +6149,7 @@
       <c r="AK65" s="3"/>
       <c r="AL65" s="3"/>
     </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6161,13 +6158,13 @@
         <v>2008</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E66" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F66">
         <v>48</v>
@@ -6182,12 +6179,12 @@
         <v>39633</v>
       </c>
       <c r="J66" s="1"/>
-      <c r="K66" s="10">
+      <c r="K66">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M66" s="5">
         <v>16.098611111111111</v>
@@ -6197,7 +6194,7 @@
       </c>
       <c r="O66" s="3"/>
       <c r="P66" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
@@ -6226,7 +6223,7 @@
       <c r="AK66" s="3"/>
       <c r="AL66" s="3"/>
     </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A85" si="2">C67&amp;B67&amp;"Cv"&amp;D67&amp;"Treat"&amp;E67</f>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6235,13 +6232,13 @@
         <v>2008</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E67" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F67">
         <v>48</v>
@@ -6256,7 +6253,7 @@
         <v>39640</v>
       </c>
       <c r="J67" s="1"/>
-      <c r="K67" s="10">
+      <c r="K67">
         <f t="shared" ref="K67:K85" si="3">I67-H67</f>
         <v>64</v>
       </c>
@@ -6308,7 +6305,7 @@
       <c r="AK67" s="3"/>
       <c r="AL67" s="3"/>
     </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6317,13 +6314,13 @@
         <v>2008</v>
       </c>
       <c r="C68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F68">
         <v>48</v>
@@ -6338,7 +6335,7 @@
         <v>39655</v>
       </c>
       <c r="J68" s="1"/>
-      <c r="K68" s="10">
+      <c r="K68">
         <f t="shared" si="3"/>
         <v>79</v>
       </c>
@@ -6390,7 +6387,7 @@
       <c r="AK68" s="3"/>
       <c r="AL68" s="3"/>
     </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6399,13 +6396,13 @@
         <v>2008</v>
       </c>
       <c r="C69" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E69" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F69">
         <v>48</v>
@@ -6420,7 +6417,7 @@
         <v>39668</v>
       </c>
       <c r="J69" s="1"/>
-      <c r="K69" s="10">
+      <c r="K69">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
@@ -6472,7 +6469,7 @@
       <c r="AK69" s="3"/>
       <c r="AL69" s="3"/>
     </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6481,13 +6478,13 @@
         <v>2008</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E70" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F70">
         <v>48</v>
@@ -6502,7 +6499,7 @@
         <v>39708</v>
       </c>
       <c r="J70" s="1"/>
-      <c r="K70" s="10">
+      <c r="K70">
         <f t="shared" si="3"/>
         <v>132</v>
       </c>
@@ -6554,7 +6551,7 @@
       <c r="AK70" s="3"/>
       <c r="AL70" s="3"/>
     </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLate</v>
@@ -6563,13 +6560,13 @@
         <v>2008</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E71" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F71">
         <v>48</v>
@@ -6583,10 +6580,10 @@
       <c r="I71" s="1">
         <v>39763</v>
       </c>
-      <c r="J71" s="10">
+      <c r="J71">
         <v>9</v>
       </c>
-      <c r="K71" s="10">
+      <c r="K71">
         <f t="shared" si="3"/>
         <v>187</v>
       </c>
@@ -6665,7 +6662,7 @@
         <v>1.1817984780042505E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6674,13 +6671,13 @@
         <v>2008</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E72" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F72">
         <v>27</v>
@@ -6695,7 +6692,7 @@
         <v>39611</v>
       </c>
       <c r="J72" s="1"/>
-      <c r="K72" s="10">
+      <c r="K72">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
@@ -6747,7 +6744,7 @@
       <c r="AK72" s="3"/>
       <c r="AL72" s="3"/>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6756,13 +6753,13 @@
         <v>2008</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E73" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73">
         <v>27</v>
@@ -6777,12 +6774,12 @@
         <v>39633</v>
       </c>
       <c r="J73" s="1"/>
-      <c r="K73" s="10">
+      <c r="K73">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L73" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M73" s="5">
         <v>41.113312499999992</v>
@@ -6827,7 +6824,7 @@
       <c r="AK73" s="3"/>
       <c r="AL73" s="3"/>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6836,13 +6833,13 @@
         <v>2008</v>
       </c>
       <c r="C74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E74" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F74">
         <v>27</v>
@@ -6857,7 +6854,7 @@
         <v>39640</v>
       </c>
       <c r="J74" s="1"/>
-      <c r="K74" s="10">
+      <c r="K74">
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
@@ -6909,7 +6906,7 @@
       <c r="AK74" s="3"/>
       <c r="AL74" s="3"/>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -6918,13 +6915,13 @@
         <v>2008</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E75" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75">
         <v>27</v>
@@ -6939,7 +6936,7 @@
         <v>39655</v>
       </c>
       <c r="J75" s="1"/>
-      <c r="K75" s="10">
+      <c r="K75">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
@@ -6991,7 +6988,7 @@
       <c r="AK75" s="3"/>
       <c r="AL75" s="3"/>
     </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -7000,13 +6997,13 @@
         <v>2008</v>
       </c>
       <c r="C76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E76" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76">
         <v>27</v>
@@ -7021,7 +7018,7 @@
         <v>39668</v>
       </c>
       <c r="J76" s="1"/>
-      <c r="K76" s="10">
+      <c r="K76">
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
@@ -7073,7 +7070,7 @@
       <c r="AK76" s="3"/>
       <c r="AL76" s="3"/>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -7082,13 +7079,13 @@
         <v>2008</v>
       </c>
       <c r="C77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77">
         <v>27</v>
@@ -7103,7 +7100,7 @@
         <v>39684</v>
       </c>
       <c r="J77" s="1"/>
-      <c r="K77" s="10">
+      <c r="K77">
         <f t="shared" si="3"/>
         <v>117</v>
       </c>
@@ -7155,7 +7152,7 @@
       <c r="AK77" s="3"/>
       <c r="AL77" s="3"/>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A78" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatLow</v>
@@ -7164,13 +7161,13 @@
         <v>2008</v>
       </c>
       <c r="C78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D78" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E78" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F78">
         <v>27</v>
@@ -7184,10 +7181,10 @@
       <c r="I78" s="1">
         <v>39749</v>
       </c>
-      <c r="J78" s="10">
+      <c r="J78">
         <v>9</v>
       </c>
-      <c r="K78" s="10">
+      <c r="K78">
         <f t="shared" si="3"/>
         <v>182</v>
       </c>
@@ -7266,7 +7263,7 @@
         <v>1.1129064835374528E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7275,13 +7272,13 @@
         <v>2008</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D79" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F79">
         <v>48</v>
@@ -7296,7 +7293,7 @@
         <v>39611</v>
       </c>
       <c r="J79" s="1"/>
-      <c r="K79" s="10">
+      <c r="K79">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
@@ -7348,7 +7345,7 @@
       <c r="AK79" s="3"/>
       <c r="AL79" s="3"/>
     </row>
-    <row r="80" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7357,13 +7354,13 @@
         <v>2008</v>
       </c>
       <c r="C80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D80" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F80">
         <v>48</v>
@@ -7378,12 +7375,12 @@
         <v>39633</v>
       </c>
       <c r="J80" s="1"/>
-      <c r="K80" s="10">
+      <c r="K80">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="M80" s="5">
         <v>79.810187500000012</v>
@@ -7428,7 +7425,7 @@
       <c r="AK80" s="3"/>
       <c r="AL80" s="3"/>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7437,13 +7434,13 @@
         <v>2008</v>
       </c>
       <c r="C81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D81" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F81">
         <v>48</v>
@@ -7458,7 +7455,7 @@
         <v>39640</v>
       </c>
       <c r="J81" s="1"/>
-      <c r="K81" s="10">
+      <c r="K81">
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
@@ -7510,7 +7507,7 @@
       <c r="AK81" s="3"/>
       <c r="AL81" s="3"/>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7519,13 +7516,13 @@
         <v>2008</v>
       </c>
       <c r="C82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D82" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82">
         <v>48</v>
@@ -7540,7 +7537,7 @@
         <v>39655</v>
       </c>
       <c r="J82" s="1"/>
-      <c r="K82" s="10">
+      <c r="K82">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
@@ -7592,7 +7589,7 @@
       <c r="AK82" s="3"/>
       <c r="AL82" s="3"/>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7601,13 +7598,13 @@
         <v>2008</v>
       </c>
       <c r="C83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83">
         <v>48</v>
@@ -7622,7 +7619,7 @@
         <v>39668</v>
       </c>
       <c r="J83" s="1"/>
-      <c r="K83" s="10">
+      <c r="K83">
         <f t="shared" si="3"/>
         <v>101</v>
       </c>
@@ -7674,7 +7671,7 @@
       <c r="AK83" s="3"/>
       <c r="AL83" s="3"/>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7683,13 +7680,13 @@
         <v>2008</v>
       </c>
       <c r="C84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D84" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84">
         <v>48</v>
@@ -7704,7 +7701,7 @@
         <v>39687</v>
       </c>
       <c r="J84" s="1"/>
-      <c r="K84" s="10">
+      <c r="K84">
         <f t="shared" si="3"/>
         <v>120</v>
       </c>
@@ -7756,7 +7753,7 @@
       <c r="AK84" s="3"/>
       <c r="AL84" s="3"/>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A85" t="str">
         <f t="shared" si="2"/>
         <v>Wagga2008CvATR_MarlinTreatMid</v>
@@ -7765,13 +7762,13 @@
         <v>2008</v>
       </c>
       <c r="C85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D85" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F85">
         <v>48</v>
@@ -7785,10 +7782,10 @@
       <c r="I85" s="1">
         <v>39749</v>
       </c>
-      <c r="J85" s="10">
+      <c r="J85">
         <v>9</v>
       </c>
-      <c r="K85" s="10">
+      <c r="K85">
         <f t="shared" si="3"/>
         <v>182</v>
       </c>
@@ -7867,21 +7864,21 @@
         <v>1.0325385711615488E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B86">
         <v>2008</v>
       </c>
       <c r="C86" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H86" s="1">
         <v>39576</v>
@@ -7931,21 +7928,21 @@
       <c r="AO86" s="2"/>
       <c r="AP86" s="2"/>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B87">
         <v>2008</v>
       </c>
       <c r="C87" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E87" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H87" s="1">
         <v>39576</v>
@@ -7995,21 +7992,21 @@
       <c r="AO87" s="2"/>
       <c r="AP87" s="2"/>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B88">
         <v>2008</v>
       </c>
       <c r="C88" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E88" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H88" s="1">
         <v>39576</v>
@@ -8059,21 +8056,21 @@
       <c r="AO88" s="2"/>
       <c r="AP88" s="2"/>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B89">
         <v>2008</v>
       </c>
       <c r="C89" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E89" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H89" s="1">
         <v>39576</v>
@@ -8123,21 +8120,21 @@
       <c r="AO89" s="2"/>
       <c r="AP89" s="2"/>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B90">
         <v>2008</v>
       </c>
       <c r="C90" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E90" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H90" s="1">
         <v>39576</v>
@@ -8191,21 +8188,21 @@
       <c r="AO90" s="2"/>
       <c r="AP90" s="2"/>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B91">
         <v>2008</v>
       </c>
       <c r="C91" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D91" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H91" s="1">
         <v>39576</v>
@@ -8255,21 +8252,21 @@
       <c r="AO91" s="2"/>
       <c r="AP91" s="2"/>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B92">
         <v>2008</v>
       </c>
       <c r="C92" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E92" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H92" s="1">
         <v>39576</v>
@@ -8319,21 +8316,21 @@
       <c r="AO92" s="2"/>
       <c r="AP92" s="2"/>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B93">
         <v>2008</v>
       </c>
       <c r="C93" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D93" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E93" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H93" s="1">
         <v>39576</v>
@@ -8383,21 +8380,21 @@
       <c r="AO93" s="2"/>
       <c r="AP93" s="2"/>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B94">
         <v>2008</v>
       </c>
       <c r="C94" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E94" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H94" s="1">
         <v>39576</v>
@@ -8447,21 +8444,21 @@
       <c r="AO94" s="2"/>
       <c r="AP94" s="2"/>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B95">
         <v>2008</v>
       </c>
       <c r="C95" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D95" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E95" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H95" s="1">
         <v>39576</v>
@@ -8515,21 +8512,21 @@
       <c r="AO95" s="2"/>
       <c r="AP95" s="2"/>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B96">
         <v>2008</v>
       </c>
       <c r="C96" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E96" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H96" s="1">
         <v>39576</v>
@@ -8579,21 +8576,21 @@
       <c r="AO96" s="2"/>
       <c r="AP96" s="2"/>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B97">
         <v>2008</v>
       </c>
       <c r="C97" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D97" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E97" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H97" s="1">
         <v>39576</v>
@@ -8643,21 +8640,21 @@
       <c r="AO97" s="2"/>
       <c r="AP97" s="2"/>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B98">
         <v>2008</v>
       </c>
       <c r="C98" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D98" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E98" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H98" s="1">
         <v>39576</v>
@@ -8702,21 +8699,21 @@
       <c r="AJ98" s="2"/>
       <c r="AK98" s="3"/>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B99">
         <v>2008</v>
       </c>
       <c r="C99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D99" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E99" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H99" s="1">
         <v>39576</v>
@@ -8761,21 +8758,21 @@
       <c r="AJ99" s="2"/>
       <c r="AK99" s="3"/>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B100">
         <v>2008</v>
       </c>
       <c r="C100" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D100" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E100" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H100" s="1">
         <v>39576</v>

</xml_diff>